<commit_message>
InteractionType, Interactive, DialogueManager 수정
InteractionType - GetType() 메소드 내부 이름 중복으로 인한 이름 수정
Interactive - GetType()메소드 이름 수정으로 같이 수정
DIalogueManager - 독백 시 DialogueNameBar 출력되지 않게 수정
New Material(빨강) -> Red 로 Material이름 변경
</commit_message>
<xml_diff>
--- a/Assets/작업일지 및 제작정리.xlsx
+++ b/Assets/작업일지 및 제작정리.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\PromiseNeverland\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A346DE-2AE3-4EFC-B80D-A1DCAB2F3817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC08382-FE4E-4CC7-A26C-5CA55EF8CED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4155" yWindow="1860" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
   <si>
     <t>날짜</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -150,10 +150,6 @@
   </si>
   <si>
     <t>[System.Serialized] DialogueEvent</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>뭔지 모름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -337,6 +333,24 @@
 DialogueManager - NextDialogue에 if(마우스좌클릭) 조건문 하나 제거;
 PlayerMovement - 물건 위에서 점프안되서 if(땅에 닿으면 점프가능) 조건문 제거;
 testDialogue.csv에 에러 메시지 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monobehavior를 상속받지 않음, 유니티 inspector창에서 이름과 대사 내용을 불러올 수 있게 만듬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화 내용의 이름(제목), 호출 줄, 대화내용의 배열의 변수 선언</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DialogueManager - SettingUI()에 독백 시 go_DialogueNameBar가 출력되지 않게 수정
+Interactive - Interact()에 있는 GetType() -&gt; GetObjectType() 으로 수정, InteractionType에서 이름을 수정했기 때문
+InteractionType - GetType() -&gt; GetObjectType() 으로 메소드 이름 수정, 내부적으로 중복된 이름이 있어서 warning이 뜬 것으로 추정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DialogueManager, Interactive, InteractionType</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -674,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D4"/>
+  <dimension ref="B2:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -714,10 +728,21 @@
         <v>220220</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>76</v>
+    </row>
+    <row r="5" spans="2:4" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>220221</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +774,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -766,7 +791,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -822,7 +847,7 @@
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -856,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
@@ -889,69 +914,75 @@
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E8" t="s">
         <v>30</v>
       </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
         <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
         <v>35</v>
-      </c>
-      <c r="F10" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
         <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
         <v>39</v>
-      </c>
-      <c r="F12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" t="s">
         <v>41</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
         <v>21</v>
@@ -960,10 +991,10 @@
         <v>22</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -995,7 +1026,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
@@ -1012,114 +1043,114 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
         <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
         <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" t="s">
         <v>60</v>
-      </c>
-      <c r="F8" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" t="s">
         <v>62</v>
-      </c>
-      <c r="F9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
         <v>64</v>
-      </c>
-      <c r="F10" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" t="s">
         <v>68</v>
-      </c>
-      <c r="F13" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>